<commit_message>
adicionando docs de dados
</commit_message>
<xml_diff>
--- a/docs/PAA-ordenacao.xlsx
+++ b/docs/PAA-ordenacao.xlsx
@@ -185,7 +185,830 @@
   </cellStyles>
   <dxfs count="55">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -303,830 +1126,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1920,24 +1920,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84651392"/>
-        <c:axId val="84654336"/>
+        <c:axId val="148178048"/>
+        <c:axId val="148179584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84651392"/>
+        <c:axId val="148178048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84654336"/>
+        <c:crossAx val="148179584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84654336"/>
+        <c:axId val="148179584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,7 +1945,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84651392"/>
+        <c:crossAx val="148178048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1958,7 +1958,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2016,24 +2016,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="B2:H14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="B2:H14" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="B2:H14"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Colunas1" dataDxfId="7"/>
-    <tableColumn id="2" name="Colunas2" dataDxfId="6"/>
-    <tableColumn id="3" name="Colunas3" dataDxfId="5"/>
-    <tableColumn id="4" name="Colunas4" dataDxfId="4"/>
-    <tableColumn id="5" name="Colunas5" dataDxfId="3"/>
-    <tableColumn id="6" name="Colunas6" dataDxfId="2"/>
-    <tableColumn id="7" name="Colunas7" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="S2:Y14" totalsRowShown="0" headerRowDxfId="46">
-  <autoFilter ref="S2:Y14"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Colunas1" dataDxfId="45"/>
     <tableColumn id="2" name="Colunas2" dataDxfId="44"/>
@@ -2047,25 +2031,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela17" displayName="Tabela17" ref="S18:Y30" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="S18:Y30"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Colunas1" dataDxfId="15"/>
-    <tableColumn id="2" name="Colunas2" dataDxfId="14"/>
-    <tableColumn id="3" name="Colunas3" dataDxfId="13"/>
-    <tableColumn id="4" name="Colunas4" dataDxfId="12"/>
-    <tableColumn id="5" name="Colunas5" dataDxfId="11"/>
-    <tableColumn id="6" name="Colunas6" dataDxfId="10"/>
-    <tableColumn id="7" name="Colunas7" dataDxfId="9"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela110" displayName="Tabela110" ref="AB2:AH14" totalsRowShown="0" headerRowDxfId="38">
-  <autoFilter ref="AB2:AH14"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela16" displayName="Tabela16" ref="S2:Y14" totalsRowShown="0" headerRowDxfId="38">
+  <autoFilter ref="S2:Y14"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Colunas1" dataDxfId="37"/>
     <tableColumn id="2" name="Colunas2" dataDxfId="36"/>
@@ -2079,33 +2047,65 @@
 </table>
 </file>
 
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela17" displayName="Tabela17" ref="S18:Y30" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="S18:Y30"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Colunas1" dataDxfId="29"/>
+    <tableColumn id="2" name="Colunas2" dataDxfId="28"/>
+    <tableColumn id="3" name="Colunas3" dataDxfId="27"/>
+    <tableColumn id="4" name="Colunas4" dataDxfId="26"/>
+    <tableColumn id="5" name="Colunas5" dataDxfId="25"/>
+    <tableColumn id="6" name="Colunas6" dataDxfId="24"/>
+    <tableColumn id="7" name="Colunas7" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela110" displayName="Tabela110" ref="AB2:AH14" totalsRowShown="0" headerRowDxfId="22">
+  <autoFilter ref="AB2:AH14"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Colunas1" dataDxfId="21"/>
+    <tableColumn id="2" name="Colunas2" dataDxfId="20"/>
+    <tableColumn id="3" name="Colunas3" dataDxfId="19"/>
+    <tableColumn id="4" name="Colunas4" dataDxfId="18"/>
+    <tableColumn id="5" name="Colunas5" dataDxfId="17"/>
+    <tableColumn id="6" name="Colunas6" dataDxfId="16"/>
+    <tableColumn id="7" name="Colunas7" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela111" displayName="Tabela111" ref="AB17:AH29" totalsRowShown="0">
   <autoFilter ref="AB17:AH29"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Colunas1" dataDxfId="30"/>
-    <tableColumn id="2" name="Colunas2" dataDxfId="29"/>
-    <tableColumn id="3" name="Colunas3" dataDxfId="28"/>
-    <tableColumn id="4" name="Colunas4" dataDxfId="27"/>
-    <tableColumn id="5" name="Colunas5" dataDxfId="26"/>
-    <tableColumn id="6" name="Colunas6" dataDxfId="25"/>
-    <tableColumn id="7" name="Colunas7" dataDxfId="24"/>
+    <tableColumn id="1" name="Colunas1" dataDxfId="14"/>
+    <tableColumn id="2" name="Colunas2" dataDxfId="13"/>
+    <tableColumn id="3" name="Colunas3" dataDxfId="12"/>
+    <tableColumn id="4" name="Colunas4" dataDxfId="11"/>
+    <tableColumn id="5" name="Colunas5" dataDxfId="10"/>
+    <tableColumn id="6" name="Colunas6" dataDxfId="9"/>
+    <tableColumn id="7" name="Colunas7" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela112" displayName="Tabela112" ref="B32:H44" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela112" displayName="Tabela112" ref="B32:H44" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B32:H44"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Colunas1" dataDxfId="22"/>
-    <tableColumn id="2" name="Colunas2" dataDxfId="21"/>
-    <tableColumn id="3" name="Colunas3" dataDxfId="20"/>
-    <tableColumn id="4" name="Colunas4" dataDxfId="19"/>
-    <tableColumn id="5" name="Colunas5" dataDxfId="18"/>
-    <tableColumn id="6" name="Colunas6" dataDxfId="17"/>
-    <tableColumn id="7" name="Colunas7" dataDxfId="16"/>
+    <tableColumn id="1" name="Colunas1" dataDxfId="6"/>
+    <tableColumn id="2" name="Colunas2" dataDxfId="5"/>
+    <tableColumn id="3" name="Colunas3" dataDxfId="4"/>
+    <tableColumn id="4" name="Colunas4" dataDxfId="3"/>
+    <tableColumn id="5" name="Colunas5" dataDxfId="2"/>
+    <tableColumn id="6" name="Colunas6" dataDxfId="1"/>
+    <tableColumn id="7" name="Colunas7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2398,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2416,8 +2416,8 @@
     <col min="13" max="13" width="9.7109375" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" customWidth="1"/>
     <col min="16" max="16" width="9.85546875" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="18" width="5.85546875" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
     <col min="21" max="21" width="9.7109375" customWidth="1"/>
     <col min="22" max="22" width="8.85546875" customWidth="1"/>

</xml_diff>